<commit_message>
added extension and some codes
</commit_message>
<xml_diff>
--- a/ExampleIG/output/CodeSystem-no-kodeverk-7010-norpat.codesystem.xlsx
+++ b/ExampleIG/output/CodeSystem-no-kodeverk-7010-norpat.codesystem.xlsx
@@ -47,7 +47,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Norsk patologikodeverk (NORPAT).</t>
+    <t>Norsk patologikodeverk (NORPAT)</t>
   </si>
   <si>
     <t>Status</t>
@@ -65,7 +65,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-02T14:52:41+01:00</t>
+    <t>2023-11-02T22:24:37+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>